<commit_message>
updates of MOVPE IKZ
</commit_message>
<xml_diff>
--- a/movpe_IKZ_Ga2O3/Substrate.xlsx
+++ b/movpe_IKZ_Ga2O3/Substrate.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="87">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -71,6 +71,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">The box number assigned by us to differentiate the delivered boxes within the same polishing batch</t>
     </r>
@@ -157,6 +158,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">An unique ID given to each substrate: 
 Ex. MgC121_4deg_P76189_10x10_B4_(BOX1)
@@ -179,6 +181,9 @@
     <t xml:space="preserve">The polishing batch number assigned by service supplier.</t>
   </si>
   <si>
+    <t xml:space="preserve">The crystal number from which the substrates are wafered. Aligned with the record of volume crystal growth department.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Company Supplier</t>
   </si>
   <si>
@@ -188,12 +193,12 @@
     <t xml:space="preserve">crystallographic orientation  [hkl]</t>
   </si>
   <si>
-    <t xml:space="preserve">The crystal number from which the substrates are wafered. Aligned with the record of volume crystal growth department.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The substrate miscut direction toward c-direction. The primary miscut angle.</t>
   </si>
   <si>
+    <t xml:space="preserve">The chrystallographic orientation of the miscut</t>
+  </si>
+  <si>
     <t xml:space="preserve">The substrate miscut direction toward b-direction. The primary miscut angle.</t>
   </si>
   <si>
@@ -224,6 +229,9 @@
     <t xml:space="preserve">Polishing Number</t>
   </si>
   <si>
+    <t xml:space="preserve">Crystal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Supplier</t>
   </si>
   <si>
@@ -233,13 +241,16 @@
     <t xml:space="preserve">Orientation</t>
   </si>
   <si>
-    <t xml:space="preserve">Crystal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscut c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscut b</t>
+    <t xml:space="preserve">Miscut b angle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscut b Orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscut c angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscut c Orientation</t>
   </si>
   <si>
     <t xml:space="preserve">Doping Level</t>
@@ -263,6 +274,9 @@
     <t xml:space="preserve">P12345</t>
   </si>
   <si>
+    <t xml:space="preserve">127</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cryscore</t>
   </si>
   <si>
@@ -272,7 +286,7 @@
     <t xml:space="preserve">001</t>
   </si>
   <si>
-    <t xml:space="preserve">127</t>
+    <t xml:space="preserve">011</t>
   </si>
   <si>
     <t xml:space="preserve">sapphire</t>
@@ -324,7 +338,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +385,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -378,16 +393,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -488,7 +493,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,10 +586,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,15 +602,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,15 +618,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -712,7 +705,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -1017,62 +1010,62 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="24" t="n">
+      <c r="B10" s="23" t="n">
         <v>45012</v>
       </c>
-      <c r="C10" s="25" t="n">
+      <c r="C10" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="D10" s="25" t="n">
+      <c r="D10" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="E10" s="25" t="n">
+      <c r="E10" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="F10" s="25" t="n">
+      <c r="F10" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="G10" s="25" t="n">
+      <c r="G10" s="24" t="n">
         <v>59</v>
       </c>
-      <c r="H10" s="25" t="n">
+      <c r="H10" s="24" t="n">
         <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="27" t="n">
+      <c r="B11" s="26" t="n">
         <v>44949</v>
       </c>
-      <c r="C11" s="25" t="n">
+      <c r="C11" s="24" t="n">
         <v>123</v>
       </c>
-      <c r="D11" s="25" t="n">
+      <c r="D11" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="E11" s="25" t="n">
+      <c r="E11" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="25" t="n">
+      <c r="F11" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="25" t="n">
+      <c r="G11" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="H11" s="25" t="n">
+      <c r="H11" s="24" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="27" t="n">
+      <c r="B12" s="26" t="n">
         <v>43757</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -1095,22 +1088,19 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="21"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23"/>
-    </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1128,10 +1118,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ31"/>
+  <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1139,37 +1129,36 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="1" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="19" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="23" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="25" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="AMH1" s="3"/>
-      <c r="AMI1" s="0"/>
+      <c r="F1" s="5"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="AMH2" s="3"/>
-      <c r="AMI2" s="0"/>
+      <c r="F2" s="7"/>
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,12 +1174,12 @@
       <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>5</v>
-      </c>
       <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1198,17 +1187,17 @@
         <v>5</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>5</v>
-      </c>
       <c r="M3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1205,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>5</v>
@@ -1225,22 +1214,26 @@
         <v>29</v>
       </c>
       <c r="R3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="28" t="s">
+      <c r="V3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="W3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="28" t="s">
+      <c r="X3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AMH3" s="3"/>
-      <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,8 +1243,8 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1264,12 +1257,12 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
-      <c r="AMH4" s="3"/>
-      <c r="AMI4" s="0"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="8" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,11 +1278,11 @@
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>9</v>
@@ -1304,11 +1297,11 @@
         <v>31</v>
       </c>
       <c r="K5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="M5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1316,85 +1309,87 @@
         <v>9</v>
       </c>
       <c r="O5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="8" t="s">
+      <c r="R5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="T5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="U5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="V5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AMH5" s="3"/>
-      <c r="AMI5" s="0"/>
+      <c r="W5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
+      <c r="F6" s="15"/>
       <c r="U6" s="16"/>
       <c r="V6" s="16"/>
-      <c r="AMH6" s="3"/>
-      <c r="AMI6" s="0"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="17" customFormat="true" ht="168.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="17" customFormat="true" ht="178.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="29" t="s">
+      <c r="J7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>45</v>
+      <c r="M7" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="N7" s="8" t="s">
         <v>45</v>
@@ -1403,379 +1398,477 @@
         <v>46</v>
       </c>
       <c r="P7" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="R7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="S7" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="T7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="U7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="T7" s="10" t="s">
+      <c r="V7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="U7" s="10" t="s">
+      <c r="W7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="V7" s="10" t="s">
+      <c r="X7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AMH7" s="3"/>
-      <c r="AMI7" s="0"/>
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
+      <c r="F8" s="19"/>
       <c r="U8" s="20"/>
       <c r="V8" s="20"/>
-      <c r="AMH8" s="3"/>
-      <c r="AMI8" s="0"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30" t="s">
-        <v>50</v>
+      <c r="A9" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>53</v>
-      </c>
       <c r="G9" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="N9" s="21" t="s">
         <v>45</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="P9" s="21" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="S9" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="U9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T9" s="22" t="s">
+      <c r="V9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="U9" s="22" t="s">
+      <c r="W9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="V9" s="22" t="s">
+      <c r="X9" s="22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="23" t="s">
+      <c r="A10" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="24" t="n">
+        <v>68</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="23" t="n">
         <v>45012</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>72</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="K10" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="T10" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="U10" s="32" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V10" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="F11" s="26" t="n">
+        <v>44949</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N10" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="31" t="s">
         <v>72</v>
-      </c>
-      <c r="O10" s="1" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q10" s="25" t="n">
-        <v>5</v>
-      </c>
-      <c r="R10" s="25" t="n">
-        <v>5</v>
-      </c>
-      <c r="S10" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="U10" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="V10" s="34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="27" t="n">
-        <v>44949</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>123</v>
       </c>
       <c r="J11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="K11" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="M11" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="T11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="U11" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="32" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="W11" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="F12" s="26" t="n">
+        <v>43757</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O11" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q11" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="R11" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="S11" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="U11" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="V11" s="34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="27" t="n">
-        <v>43757</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>145</v>
+      <c r="I12" s="31" t="s">
+        <v>72</v>
       </c>
       <c r="J12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K12" s="1" t="n">
+      <c r="K12" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L12" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="31" t="s">
         <v>73</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="O12" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q12" s="1" t="n">
         <v>0.012</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q12" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="R12" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="S12" s="34" t="b">
+      <c r="R12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="U12" s="32" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="T12" s="34" t="b">
+      <c r="V12" s="32" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U12" s="34" t="b">
+      <c r="W12" s="32" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V12" s="34" t="b">
+      <c r="X12" s="32" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="H13" s="35"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="I13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="M13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="H14" s="35"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="I14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="M14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="35"/>
+      <c r="I15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="M15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="35"/>
+      <c r="I16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="35"/>
+      <c r="I17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="M17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="35"/>
+      <c r="I18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="M18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="35"/>
+      <c r="I19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="M19" s="31"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="35"/>
+      <c r="I20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="M20" s="31"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="35"/>
+      <c r="I21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="M21" s="31"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="35"/>
+      <c r="I22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="M22" s="31"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="35"/>
+      <c r="I23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="M23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="35"/>
+      <c r="I24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="M24" s="31"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="35"/>
+      <c r="I25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="M25" s="31"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="35"/>
+      <c r="I26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="M26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="35"/>
+      <c r="I27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="M27" s="31"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="35"/>
+      <c r="I28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="M28" s="31"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="35"/>
+      <c r="I29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="M29" s="31"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="35"/>
+      <c r="I30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="M30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="35"/>
+      <c r="I31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="M31" s="31"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K32" s="31"/>
+      <c r="M32" s="31"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K37" s="31"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K38" s="31"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G10:G89" type="list">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H10:H89" type="list">
       <formula1>"semi-insulating,conductive"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>